<commit_message>
fix(ExcelMapper): some rows not mapped Rows having secondary-key columns with empty values are ignored;
</commit_message>
<xml_diff>
--- a/pub/publicTestData_small_onlyOneKeyColumn.xlsx
+++ b/pub/publicTestData_small_onlyOneKeyColumn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpr/dev/pubcore/vite-storybook-mui/pub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B27EA4-B7C1-CE4F-8E58-F1C15EA29BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D66F686-DF4C-4C4C-9AB1-C7CE9313F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="375">
   <si>
     <t>City</t>
   </si>
@@ -1143,13 +1143,19 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>Optional empty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1164,6 +1170,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1225,7 +1237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1235,6 +1247,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1644,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8002,71 +8015,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E4C286-C226-E44C-9644-6F71421CA926}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" t="s">
         <v>364</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>369</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>370</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>371</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C2" t="s">
         <v>368</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>369</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>370</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>371</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>366</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>367</v>
       </c>
     </row>

</xml_diff>